<commit_message>
Erros out in tcp
</commit_message>
<xml_diff>
--- a/firmware/Contrrol/Map Registers Control_LED.xlsx
+++ b/firmware/Contrrol/Map Registers Control_LED.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E338A712-08F0-4ED3-8DC6-01D91EE45628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813ECBA2-CF17-4800-A19A-3A50213F68B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
   <si>
     <t>Десятичная</t>
   </si>
@@ -183,6 +183,86 @@
   </si>
   <si>
     <t xml:space="preserve">ток канала </t>
+  </si>
+  <si>
+    <t>Delet dev</t>
+  </si>
+  <si>
+    <t>Удаление девайса из памяти</t>
+  </si>
+  <si>
+    <t>is on</t>
+  </si>
+  <si>
+    <t>включен ли каннал</t>
+  </si>
+  <si>
+    <t>PWM read</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>load in flash</t>
+  </si>
+  <si>
+    <t>Reboot</t>
+  </si>
+  <si>
+    <t>младший байт ip загружаем из флешки или из переключателей</t>
+  </si>
+  <si>
+    <t>ip</t>
+  </si>
+  <si>
+    <t>gw</t>
+  </si>
+  <si>
+    <t>mac</t>
+  </si>
+  <si>
+    <t>C1A16D1N1x
+C11 - комманда
+A1 - какую часть адреса пишем 192.168.1.100
+192(4) 168(3) 1(2) 100(1) 
+D -значение для установки
+N1 - не используется</t>
+  </si>
+  <si>
+    <t>C1A1D192N0x
+C11 - комманда
+A1 - какую часть адреса пишем 192.168.1.100
+192(4) 168(3) 1(2) 100(1) 
+D -значение для установки
+N1 - не используется</t>
+  </si>
+  <si>
+    <t>C1A1D255N0x
+C11 - комманда
+A1 - какую часть адреса пишем 255.255.255.0
+255(4) 255(3) 255(2) 0(1) 
+D -значение для установки
+N1 - не используется</t>
+  </si>
+  <si>
+    <t>C1A16D1N1x
+C11 - комманда
+A1 - какую часть адреса пишем xx.xx.xx.xx.xx.xx
+xx(6) xx(5) xx(4) xx(3) xx(2) xx(1) 
+D -значение для установки
+N1 - не используется</t>
+  </si>
+  <si>
+    <t>установка мак адреса</t>
+  </si>
+  <si>
+    <t>установка шлюза</t>
+  </si>
+  <si>
+    <t>DHCP</t>
+  </si>
+  <si>
+    <t>Включение или выключение DHCP</t>
   </si>
   <si>
     <r>
@@ -235,7 +315,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> - адрес устройства в десятичной системе
-16 + число установленное перемычками от 16 до 31 включительно
+число 16 + число установленное перемычками итоговое число от 16 до 31 включительно
 </t>
     </r>
     <r>
@@ -287,26 +367,23 @@
     </r>
   </si>
   <si>
-    <t>Delet dev</t>
-  </si>
-  <si>
-    <t>Удаление девайса из памяти</t>
-  </si>
-  <si>
-    <t>is on</t>
-  </si>
-  <si>
-    <t>включен ли каннал</t>
-  </si>
-  <si>
-    <t>PWM read</t>
+    <t>mask</t>
+  </si>
+  <si>
+    <t>маска</t>
+  </si>
+  <si>
+    <t>ip адрес</t>
+  </si>
+  <si>
+    <t>Get errors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +411,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -704,7 +788,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -724,9 +808,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -796,6 +877,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1146,8 +1233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BI49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1156,24 +1243,24 @@
     <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5546875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="41.44140625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="41.44140625" style="23" customWidth="1"/>
     <col min="7" max="7" width="25.5546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.88671875" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E1" s="16"/>
-      <c r="F1" s="21"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:7" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:7" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -1185,228 +1272,258 @@
       <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="162.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="27">
         <v>1</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="22" t="s">
+      <c r="E4" s="27"/>
+      <c r="F4" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="33">
+        <v>2</v>
+      </c>
+      <c r="C5" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="22"/>
-    </row>
-    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+      <c r="D5" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+    </row>
+    <row r="6" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="33">
+        <v>3</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+    </row>
+    <row r="7" spans="1:7" s="26" customFormat="1" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="33">
+        <v>4</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="33">
         <v>5</v>
       </c>
-      <c r="B5" s="34">
-        <v>2</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="34" t="s">
+      <c r="C8" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+    </row>
+    <row r="9" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="33">
+        <v>6</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="33">
+        <v>7</v>
+      </c>
+      <c r="C10" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-    </row>
-    <row r="6" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="34">
-        <v>3</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-    </row>
-    <row r="7" spans="1:7" s="27" customFormat="1" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="34">
-        <v>4</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
+      <c r="D10" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="33">
         <v>8</v>
       </c>
-      <c r="B8" s="34">
-        <v>5</v>
-      </c>
-      <c r="C8" s="34" t="s">
+      <c r="C11" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-    </row>
-    <row r="9" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="34" t="s">
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+    </row>
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="33">
         <v>9</v>
       </c>
-      <c r="B9" s="34">
-        <v>6</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="34" t="s">
+      <c r="C12" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="35"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="35"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="33">
         <v>10</v>
       </c>
-      <c r="B10" s="34">
-        <v>7</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
+      <c r="C13" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+    </row>
+    <row r="14" spans="1:7" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="33">
         <v>11</v>
       </c>
-      <c r="B11" s="34">
-        <v>8</v>
-      </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="34" t="s">
+      <c r="C14" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+    </row>
+    <row r="15" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="33">
         <v>12</v>
       </c>
-      <c r="B12" s="34">
-        <v>9</v>
-      </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="36"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="34" t="s">
+      <c r="C15" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="33"/>
+    </row>
+    <row r="16" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="33">
         <v>13</v>
       </c>
-      <c r="B13" s="34">
-        <v>10</v>
-      </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="34" t="s">
+      <c r="C16" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="33"/>
+    </row>
+    <row r="17" spans="1:61" s="3" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="33">
         <v>14</v>
       </c>
-      <c r="B14" s="34">
-        <v>11</v>
-      </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="34">
-        <v>12</v>
-      </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="34">
-        <v>13</v>
-      </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-    </row>
-    <row r="17" spans="1:61" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="34">
-        <v>14</v>
-      </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
+      <c r="C17" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="33"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1462,57 +1579,65 @@
       <c r="BH17" s="2"/>
       <c r="BI17" s="2"/>
     </row>
-    <row r="18" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+    <row r="18" spans="1:61" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="34">
+      <c r="B18" s="33">
         <v>15</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
+      <c r="C18" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="33"/>
     </row>
     <row r="19" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="34">
+      <c r="B19" s="33">
         <v>16</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
+      <c r="C19" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
     </row>
     <row r="20" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="34">
+      <c r="B20" s="33">
         <v>17</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="31">
         <v>18</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="10"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
@@ -1521,11 +1646,11 @@
       <c r="B22" s="6">
         <v>19</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="11"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
@@ -1534,11 +1659,11 @@
       <c r="B23" s="6">
         <v>20</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="11"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
@@ -1547,11 +1672,11 @@
       <c r="B24" s="7">
         <v>21</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="11"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
@@ -1560,11 +1685,11 @@
       <c r="B25" s="6">
         <v>22</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="11"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
@@ -1573,11 +1698,11 @@
       <c r="B26" s="6">
         <v>23</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="11"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="10"/>
     </row>
     <row r="27" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
@@ -1586,11 +1711,11 @@
       <c r="B27" s="7">
         <v>24</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="11"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
@@ -1599,11 +1724,11 @@
       <c r="B28" s="6">
         <v>25</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="11"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
@@ -1612,11 +1737,11 @@
       <c r="B29" s="6">
         <v>26</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="11"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="10"/>
     </row>
     <row r="30" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
@@ -1625,11 +1750,11 @@
       <c r="B30" s="6">
         <v>27</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="11"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="10"/>
     </row>
     <row r="31" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
@@ -1638,11 +1763,11 @@
       <c r="B31" s="7">
         <v>28</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="11"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="10"/>
     </row>
     <row r="32" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
@@ -1651,11 +1776,11 @@
       <c r="B32" s="6">
         <v>29</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="11"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="10"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
@@ -1664,11 +1789,11 @@
       <c r="B33" s="6">
         <v>30</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="11"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
@@ -1677,11 +1802,11 @@
       <c r="B34" s="6">
         <v>31</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="11"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="10"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
@@ -1690,11 +1815,11 @@
       <c r="B35" s="6">
         <v>32</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="11"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
@@ -1703,11 +1828,11 @@
       <c r="B36" s="6">
         <v>33</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="11"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="10"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
@@ -1716,11 +1841,11 @@
       <c r="B37" s="6">
         <v>34</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="11"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="10"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
@@ -1729,11 +1854,11 @@
       <c r="B38" s="6">
         <v>35</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="11"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="10"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
@@ -1742,11 +1867,11 @@
       <c r="B39" s="7">
         <v>36</v>
       </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="11"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="10"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
@@ -1755,11 +1880,11 @@
       <c r="B40" s="6">
         <v>37</v>
       </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="11"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="10"/>
     </row>
     <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
@@ -1768,11 +1893,11 @@
       <c r="B41" s="6">
         <v>38</v>
       </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="11"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="10"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
@@ -1781,11 +1906,11 @@
       <c r="B42" s="6">
         <v>39</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="11"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="10"/>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
@@ -1794,11 +1919,11 @@
       <c r="B43" s="6">
         <v>40</v>
       </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="11"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="10"/>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
@@ -1807,11 +1932,11 @@
       <c r="B44" s="6">
         <v>41</v>
       </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="11"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="10"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
@@ -1820,11 +1945,11 @@
       <c r="B45" s="6">
         <v>42</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="11"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
@@ -1833,11 +1958,11 @@
       <c r="B46" s="6">
         <v>43</v>
       </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="11"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
@@ -1846,11 +1971,11 @@
       <c r="B47" s="7">
         <v>44</v>
       </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="11"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="10"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
@@ -1859,11 +1984,11 @@
       <c r="B48" s="6">
         <v>45</v>
       </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="11"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="8" t="s">
@@ -1872,11 +1997,11 @@
       <c r="B49" s="6">
         <v>46</v>
       </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="11"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
changed communication I2C to UART
</commit_message>
<xml_diff>
--- a/firmware/Contrrol/Map Registers Control_LED.xlsx
+++ b/firmware/Contrrol/Map Registers Control_LED.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374D5D44-82BA-4AA0-89C6-0CA9A9349965}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834D963C-69CA-48E0-A16E-18FA250B0055}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -386,6 +386,208 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">C1A0D1000N0x
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - комманда
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">D_ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Шим на канал
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - имя канала, число от 0 до 47  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C1A16D1N0x
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - комманда
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">D_ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- 0 выключить 1 включить
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - имя канала, число от 0 до 47  </t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">C1A16D1N1x
 </t>
     </r>
@@ -434,7 +636,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - Адрес начала диапазонм. начинается от 16
+      <t xml:space="preserve"> - Адрес начала диапазона. начинается с 1
 </t>
     </r>
     <r>
@@ -486,208 +688,6 @@
  записывать "0"
  читать"1" 
  очистить память устройств "2"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">C1A16D1N1x
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - комманда
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>A0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> -
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">D_ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- Шим на канал
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - имя канала, число от 0 до 47  </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">C1A16D1N1x
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - комманда
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>A0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> -  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">D_ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- 0 выключить 1 включить
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - имя канала, число от 0 до 47  </t>
     </r>
   </si>
 </sst>
@@ -1545,8 +1545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BI49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1556,8 +1556,8 @@
     <col min="3" max="3" width="18.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="27.5546875" style="18" customWidth="1"/>
-    <col min="6" max="6" width="41.44140625" style="23" customWidth="1"/>
-    <col min="7" max="7" width="25.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43.88671875" style="23" customWidth="1"/>
+    <col min="7" max="7" width="43.88671875" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.88671875" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -1612,7 +1612,7 @@
       </c>
       <c r="E4" s="33"/>
       <c r="F4" s="21" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G4" s="33"/>
     </row>
@@ -1667,7 +1667,7 @@
       </c>
       <c r="E7" s="33"/>
       <c r="F7" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G7" s="33"/>
     </row>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="E8" s="33"/>
       <c r="F8" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G8" s="33"/>
     </row>

</xml_diff>